<commit_message>
Updating table 1 to have number of observations in data. Adding prevalences
</commit_message>
<xml_diff>
--- a/Tables/tables.xlsx
+++ b/Tables/tables.xlsx
@@ -7,16 +7,17 @@
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId2"/>
-    <sheet name="Univariate Regression" sheetId="2" r:id="rId4"/>
-    <sheet name="Periodontal Stage Regression" sheetId="3" r:id="rId5"/>
-    <sheet name="Oral Health Regression" sheetId="4" r:id="rId6"/>
+    <sheet name="Prevalence" sheetId="2" r:id="rId4"/>
+    <sheet name="Univariate Regression" sheetId="3" r:id="rId5"/>
+    <sheet name="Periodontal Stage Regression" sheetId="4" r:id="rId6"/>
+    <sheet name="Oral Health Regression" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="227">
   <si>
     <t>Periodontal Disease</t>
   </si>
@@ -36,7 +37,10 @@
     <t>p-value</t>
   </si>
   <si>
-    <t>Number of Patients</t>
+    <t>Number of observations</t>
+  </si>
+  <si>
+    <t>Equivalent population number</t>
   </si>
   <si>
     <t>Age in years (S.D.)</t>
@@ -196,6 +200,24 @@
   </si>
   <si>
     <t>158.5 (241.6)</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>CAD and/or Stroke</t>
+  </si>
+  <si>
+    <t>Periodontal disease stage</t>
+  </si>
+  <si>
+    <t>Stage 1</t>
+  </si>
+  <si>
+    <t>Stage 2</t>
+  </si>
+  <si>
+    <t>Stage 3 – Stage 4</t>
   </si>
   <si>
     <t>Variable</t>
@@ -682,10 +704,27 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="166" formatCode="#.#"/>
+    <numFmt numFmtId="167" formatCode="#.##"/>
   </numFmts>
-  <fonts count="49">
+  <fonts count="53">
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -891,7 +930,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="49">
+  <borders count="53">
     <border>
       <left/>
       <right/>
@@ -1235,11 +1274,39 @@
       <bottom style="none"/>
       <diagonal style="none"/>
     </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
@@ -1430,6 +1497,22 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="48" fillId="0" borderId="48" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="49" fillId="0" borderId="49" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="50" fillId="0" borderId="50" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="51" fillId="0" borderId="51" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="52" fillId="0" borderId="52" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1442,7 +1525,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E30"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -1472,431 +1555,445 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>20018621.560837995</v>
+        <v>358</v>
       </c>
       <c r="C3">
-        <v>68658090.833549008</v>
+        <v>1532</v>
       </c>
       <c r="D3">
-        <v>30924972.590289</v>
+        <v>939</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4">
-        <v>4.1939950098300001e-08</v>
+      <c r="B4">
+        <v>20018621.560837995</v>
+      </c>
+      <c r="C4">
+        <v>68658090.833548993</v>
+      </c>
+      <c r="D4">
+        <v>30924972.590289</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="1">
-        <v>36.019368685473864</v>
-      </c>
-      <c r="C5" s="2">
-        <v>49.709185122826149</v>
-      </c>
-      <c r="D5" s="3">
-        <v>59.925552488054144</v>
-      </c>
       <c r="E5">
-        <v>1.82236331547e-09</v>
+        <v>4.1939950098300001e-08</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="4">
-        <v>80.963297070417909</v>
-      </c>
-      <c r="C6" s="5">
-        <v>70.929777882875172</v>
-      </c>
-      <c r="D6" s="6">
-        <v>58.88079200129642</v>
+      <c r="B6" s="1">
+        <v>36.019368685473871</v>
+      </c>
+      <c r="C6" s="2">
+        <v>49.709185122826163</v>
+      </c>
+      <c r="D6" s="3">
+        <v>59.925552488054137</v>
       </c>
       <c r="E6">
-        <v>2.3955042875599999e-06</v>
+        <v>1.82236331547e-09</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="7">
-        <v>90.819537101514243</v>
-      </c>
-      <c r="C7" s="8">
-        <v>86.069460949994209</v>
-      </c>
-      <c r="D7" s="9">
-        <v>83.935257549540864</v>
+      <c r="B7" s="4">
+        <v>80.963297070417923</v>
+      </c>
+      <c r="C7" s="5">
+        <v>70.929777882875172</v>
+      </c>
+      <c r="D7" s="6">
+        <v>58.88079200129642</v>
       </c>
       <c r="E7">
-        <v>0.0145336946862312</v>
+        <v>2.3955042875599999e-06</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="10">
-        <v>19.7622933440148</v>
-      </c>
-      <c r="C8" s="11">
-        <v>27.498233629752523</v>
-      </c>
-      <c r="D8" s="12">
-        <v>52.453095926958781</v>
+      <c r="B8" s="7">
+        <v>90.819537101514243</v>
+      </c>
+      <c r="C8" s="8">
+        <v>86.069460949994223</v>
+      </c>
+      <c r="D8" s="9">
+        <v>83.935257549540907</v>
       </c>
       <c r="E8">
-        <v>2.8990348247599998e-10</v>
+        <v>0.0145336946862312</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
         <v>15</v>
       </c>
+      <c r="B9" s="10">
+        <v>19.762293344014804</v>
+      </c>
+      <c r="C9" s="11">
+        <v>27.498233629752516</v>
+      </c>
+      <c r="D9" s="12">
+        <v>52.453095926958781</v>
+      </c>
       <c r="E9">
-        <v>2.53980863326e-11</v>
+        <v>2.8990348247599998e-10</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="13">
-        <v>6.274937587882631</v>
-      </c>
-      <c r="C10" s="14">
-        <v>11.256195950459867</v>
-      </c>
-      <c r="D10" s="15">
-        <v>22.485014492085661</v>
+      <c r="E10">
+        <v>2.53980863326e-11</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="16">
-        <v>8.0456842269742044</v>
-      </c>
-      <c r="C11" s="17">
-        <v>14.295688514472843</v>
-      </c>
-      <c r="D11" s="18">
-        <v>21.79073942031269</v>
+      <c r="B11" s="13">
+        <v>6.2749375878826301</v>
+      </c>
+      <c r="C11" s="14">
+        <v>11.256195950459871</v>
+      </c>
+      <c r="D11" s="15">
+        <v>22.485014492085664</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="19">
-        <v>12.003012017149173</v>
-      </c>
-      <c r="C12" s="20">
-        <v>17.428623894980007</v>
-      </c>
-      <c r="D12" s="21">
-        <v>24.645744436596033</v>
+      <c r="B12" s="16">
+        <v>8.0456842269742026</v>
+      </c>
+      <c r="C12" s="17">
+        <v>14.295688514472848</v>
+      </c>
+      <c r="D12" s="18">
+        <v>21.79073942031269</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="22">
-        <v>6.8233001301505256</v>
-      </c>
-      <c r="C13" s="23">
-        <v>7.7126595588024704</v>
-      </c>
-      <c r="D13" s="24">
-        <v>6.6562966618388941</v>
+      <c r="B13" s="19">
+        <v>12.003012017149169</v>
+      </c>
+      <c r="C13" s="20">
+        <v>17.42862389498001</v>
+      </c>
+      <c r="D13" s="21">
+        <v>24.645744436596033</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="25">
-        <v>66.85306603784349</v>
-      </c>
-      <c r="C14" s="26">
-        <v>49.306832081284796</v>
-      </c>
-      <c r="D14" s="27">
-        <v>24.422204989166712</v>
+      <c r="B14" s="22">
+        <v>6.8233001301505238</v>
+      </c>
+      <c r="C14" s="23">
+        <v>7.7126595588024704</v>
+      </c>
+      <c r="D14" s="24">
+        <v>6.656296661838895</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
         <v>21</v>
       </c>
-      <c r="B15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E15">
-        <v>0.1154168034904879</v>
+      <c r="B15" s="25">
+        <v>66.853066037843476</v>
+      </c>
+      <c r="C15" s="26">
+        <v>49.30683208128481</v>
+      </c>
+      <c r="D15" s="27">
+        <v>24.422204989166712</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" t="s">
         <v>25</v>
       </c>
-      <c r="B16" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" t="s">
-        <v>28</v>
-      </c>
       <c r="E16">
-        <v>8.3696694410099998e-05</v>
+        <v>0.1154168034904879</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" t="s">
         <v>29</v>
       </c>
-      <c r="B17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" t="s">
-        <v>32</v>
-      </c>
       <c r="E17">
-        <v>0.96245040067693166</v>
+        <v>8.3696694410099998e-05</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="28">
-        <v>0.98031282256171992</v>
-      </c>
-      <c r="C18" s="29">
-        <v>4.3830095211612621</v>
-      </c>
-      <c r="D18" s="30">
-        <v>8.8265147755640783</v>
-      </c>
       <c r="E18">
-        <v>5.0841416421400004e-06</v>
+        <v>0.96245040067693144</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="31">
-        <v>10.428423852749081</v>
-      </c>
-      <c r="C19" s="32">
-        <v>14.245187131008718</v>
-      </c>
-      <c r="D19" s="33">
-        <v>27.465869590400899</v>
+      <c r="B19" s="28">
+        <v>0.98031282256172014</v>
+      </c>
+      <c r="C19" s="29">
+        <v>4.383009521161263</v>
+      </c>
+      <c r="D19" s="30">
+        <v>8.8265147755640783</v>
       </c>
       <c r="E19">
-        <v>1.05640650205e-05</v>
+        <v>5.0841416421400004e-06</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="34">
-        <v>5.2208564541356441</v>
-      </c>
-      <c r="C20" s="35">
-        <v>9.4176575774321858</v>
-      </c>
-      <c r="D20" s="36">
-        <v>17.873816240392486</v>
+      <c r="B20" s="31">
+        <v>10.428423852749082</v>
+      </c>
+      <c r="C20" s="32">
+        <v>14.245187131008722</v>
+      </c>
+      <c r="D20" s="33">
+        <v>27.465869590400892</v>
       </c>
       <c r="E20">
-        <v>0.00031247913670800001</v>
+        <v>1.05640650205e-05</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="37">
-        <v>19.800777953250194</v>
-      </c>
-      <c r="C21" s="38">
-        <v>29.716974905511435</v>
-      </c>
-      <c r="D21" s="39">
-        <v>38.006678243698182</v>
+      <c r="B21" s="34">
+        <v>5.2208564541356441</v>
+      </c>
+      <c r="C21" s="35">
+        <v>9.4176575774321876</v>
+      </c>
+      <c r="D21" s="36">
+        <v>17.873816240392486</v>
       </c>
       <c r="E21">
-        <v>6.4537351217000004e-05</v>
+        <v>0.00031247913670800001</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="40">
-        <v>29.498439575941493</v>
-      </c>
-      <c r="C22" s="41">
-        <v>44.078339135438966</v>
-      </c>
-      <c r="D22" s="42">
-        <v>36.438502438102702</v>
+      <c r="B22" s="37">
+        <v>19.800777953250194</v>
+      </c>
+      <c r="C22" s="38">
+        <v>29.716974905511439</v>
+      </c>
+      <c r="D22" s="39">
+        <v>38.00667824369819</v>
       </c>
       <c r="E22">
-        <v>0.0212862510209735</v>
+        <v>6.4537351217000004e-05</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
         <v>38</v>
       </c>
-      <c r="B23" t="s">
-        <v>39</v>
-      </c>
-      <c r="C23" t="s">
-        <v>40</v>
-      </c>
-      <c r="D23" t="s">
-        <v>41</v>
+      <c r="B23" s="40">
+        <v>29.4984395759415</v>
+      </c>
+      <c r="C23" s="41">
+        <v>44.078339135438966</v>
+      </c>
+      <c r="D23" s="42">
+        <v>36.438502438102702</v>
       </c>
       <c r="E23">
-        <v>0.3072257780653766</v>
+        <v>0.0212862510209735</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" t="s">
         <v>42</v>
       </c>
-      <c r="B24" t="s">
-        <v>43</v>
-      </c>
-      <c r="C24" t="s">
-        <v>44</v>
-      </c>
-      <c r="D24" t="s">
-        <v>45</v>
-      </c>
       <c r="E24">
-        <v>0.64826139543645045</v>
+        <v>0.30722577806537649</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" t="s">
+        <v>45</v>
+      </c>
+      <c r="D25" t="s">
         <v>46</v>
       </c>
-      <c r="B25" t="s">
-        <v>47</v>
-      </c>
-      <c r="C25" t="s">
-        <v>48</v>
-      </c>
-      <c r="D25" t="s">
-        <v>49</v>
-      </c>
       <c r="E25">
-        <v>0.22700401259580849</v>
+        <v>0.64826139543645089</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" t="s">
         <v>50</v>
       </c>
-      <c r="B26" t="s">
-        <v>51</v>
-      </c>
-      <c r="C26" t="s">
-        <v>52</v>
-      </c>
-      <c r="D26" t="s">
-        <v>53</v>
-      </c>
       <c r="E26">
-        <v>0.072054543945373806</v>
+        <v>0.22700401259580841</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" t="s">
+        <v>53</v>
+      </c>
+      <c r="D27" t="s">
         <v>54</v>
       </c>
-      <c r="B27" s="43">
-        <v>1.3756682953572554</v>
-      </c>
-      <c r="C27" s="44">
-        <v>1.8923904114518746</v>
-      </c>
-      <c r="D27" s="45">
-        <v>3.4715684404652434</v>
-      </c>
       <c r="E27">
-        <v>0.15175614800425291</v>
+        <v>0.072054543945374305</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
         <v>55</v>
       </c>
-      <c r="B28" s="46">
-        <v>80.834260782911798</v>
-      </c>
-      <c r="C28" s="47">
-        <v>79.287644903283237</v>
-      </c>
-      <c r="D28" s="48">
-        <v>77.239573927838279</v>
+      <c r="B28" s="43">
+        <v>1.375668295357255</v>
+      </c>
+      <c r="C28" s="44">
+        <v>1.8923904114518755</v>
+      </c>
+      <c r="D28" s="45">
+        <v>3.4715684404652425</v>
       </c>
       <c r="E28">
-        <v>0.60795178902118963</v>
+        <v>0.15175614800425291</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
         <v>56</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="46">
+        <v>80.834260782911798</v>
+      </c>
+      <c r="C29" s="47">
+        <v>79.287644903283294</v>
+      </c>
+      <c r="D29" s="48">
+        <v>77.239573927838293</v>
+      </c>
+      <c r="E29">
+        <v>0.60795178902118785</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
         <v>57</v>
       </c>
-      <c r="C29" t="s">
+      <c r="B30" t="s">
         <v>58</v>
       </c>
-      <c r="D29" t="s">
+      <c r="C30" t="s">
         <v>59</v>
       </c>
-      <c r="E29">
-        <v>0.044688020129488602</v>
+      <c r="D30" t="s">
+        <v>60</v>
+      </c>
+      <c r="E30">
+        <v>0.044688020129488401</v>
       </c>
     </row>
   </sheetData>
@@ -1905,289 +2002,45 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:D5"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B1" t="s">
         <v>61</v>
-      </c>
-      <c r="C1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C2">
-        <v>0.050727776549869999</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B3" t="s">
-        <v>65</v>
+        <v>62</v>
+      </c>
+      <c r="B2" s="49">
+        <v>4.9624159125554463</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" t="s">
         <v>66</v>
       </c>
-      <c r="B4" t="s">
-        <v>67</v>
-      </c>
     </row>
     <row r="5">
-      <c r="A5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>72</v>
-      </c>
-      <c r="B7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>74</v>
-      </c>
-      <c r="C8">
-        <v>0.00063336903912150004</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>75</v>
-      </c>
-      <c r="B9" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>77</v>
-      </c>
-      <c r="B10" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>79</v>
-      </c>
-      <c r="B11" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>81</v>
-      </c>
-      <c r="B12" t="s">
-        <v>82</v>
-      </c>
-      <c r="C12">
-        <v>3.0138811679399997e-08</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>83</v>
-      </c>
-      <c r="B13" t="s">
-        <v>84</v>
-      </c>
-      <c r="C13">
-        <v>0.47933801402904541</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>85</v>
-      </c>
-      <c r="B14" t="s">
-        <v>86</v>
-      </c>
-      <c r="C14">
-        <v>0.00014503412337480001</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>87</v>
-      </c>
-      <c r="B15" t="s">
-        <v>88</v>
-      </c>
-      <c r="C15">
-        <v>0.0028310528606144002</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s">
-        <v>89</v>
-      </c>
-      <c r="B16" t="s">
-        <v>90</v>
-      </c>
-      <c r="C16">
-        <v>0.010184494555970199</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s">
-        <v>91</v>
-      </c>
-      <c r="C17">
-        <v>0.0002826496369742</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
-        <v>92</v>
-      </c>
-      <c r="B18" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s">
-        <v>94</v>
-      </c>
-      <c r="B19" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s">
-        <v>96</v>
-      </c>
-      <c r="B20" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s">
-        <v>98</v>
-      </c>
-      <c r="B21" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s">
-        <v>100</v>
-      </c>
-      <c r="B22" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s">
-        <v>102</v>
-      </c>
-      <c r="B23" t="s">
-        <v>103</v>
-      </c>
-      <c r="C23">
-        <v>0.22084386462824951</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s">
-        <v>104</v>
-      </c>
-      <c r="B24" t="s">
-        <v>105</v>
-      </c>
-      <c r="C24">
-        <v>0.1310905020089069</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="s">
-        <v>106</v>
-      </c>
-      <c r="B25" t="s">
-        <v>107</v>
-      </c>
-      <c r="C25">
-        <v>4.3704862418200001e-07</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="s">
-        <v>108</v>
-      </c>
-      <c r="B26" t="s">
-        <v>109</v>
-      </c>
-      <c r="C26">
-        <v>5.6407893339e-06</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="s">
-        <v>110</v>
-      </c>
-      <c r="B27" t="s">
-        <v>111</v>
-      </c>
-      <c r="C27">
-        <v>0.00076361063500770003</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="s">
-        <v>112</v>
-      </c>
-      <c r="B28" t="s">
-        <v>113</v>
-      </c>
-      <c r="C28">
-        <v>3.4435466830600002e-06</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="s">
-        <v>114</v>
-      </c>
-      <c r="B29" t="s">
-        <v>115</v>
-      </c>
-      <c r="C29">
-        <v>0.52401780687608601</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="s">
-        <v>116</v>
-      </c>
-      <c r="B30" t="s">
-        <v>117</v>
-      </c>
-      <c r="C30">
-        <v>0.14909696686314869</v>
+      <c r="B5" s="50">
+        <v>16.737742083987275</v>
+      </c>
+      <c r="C5" s="51">
+        <v>57.405621703695765</v>
+      </c>
+      <c r="D5" s="52">
+        <v>25.856636212316975</v>
       </c>
     </row>
   </sheetData>
@@ -2196,272 +2049,289 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C30"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>118</v>
+        <v>67</v>
       </c>
       <c r="B1" t="s">
-        <v>119</v>
+        <v>68</v>
       </c>
       <c r="C1" t="s">
-        <v>120</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>121</v>
+        <v>70</v>
       </c>
       <c r="C2">
-        <v>0.10020741828660749</v>
+        <v>0.050727776549869701</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>122</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
-        <v>123</v>
-      </c>
-      <c r="C3"/>
+        <v>72</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>124</v>
+        <v>73</v>
       </c>
       <c r="B4" t="s">
-        <v>125</v>
-      </c>
-      <c r="C4">
-        <v>0.055103058469376416</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>126</v>
+        <v>75</v>
       </c>
       <c r="B5" t="s">
-        <v>127</v>
-      </c>
-      <c r="C5">
-        <v>0.029033502141471754</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>128</v>
+        <v>77</v>
       </c>
       <c r="B6" t="s">
-        <v>129</v>
-      </c>
-      <c r="C6">
-        <v>4.7321178266967507e-06</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>130</v>
+        <v>79</v>
       </c>
       <c r="B7" t="s">
-        <v>131</v>
-      </c>
-      <c r="C7">
-        <v>0.45929648773349718</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>132</v>
-      </c>
-      <c r="B8" t="s">
-        <v>133</v>
+        <v>81</v>
       </c>
       <c r="C8">
-        <v>0.0010867068304195569</v>
+        <v>0.00063336903912139997</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>134</v>
+        <v>82</v>
       </c>
       <c r="B9" t="s">
-        <v>135</v>
-      </c>
-      <c r="C9">
-        <v>0.042086490986395893</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>136</v>
+        <v>84</v>
       </c>
       <c r="B10" t="s">
-        <v>137</v>
-      </c>
-      <c r="C10">
-        <v>0.35067052824028389</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>138</v>
-      </c>
-      <c r="C11">
-        <v>0.29149630622275657</v>
+        <v>86</v>
+      </c>
+      <c r="B11" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>139</v>
+        <v>88</v>
       </c>
       <c r="B12" t="s">
-        <v>140</v>
+        <v>89</v>
       </c>
       <c r="C12">
-        <v>0.032963613244158675</v>
+        <v>3.0138811679399997e-08</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>141</v>
+        <v>90</v>
       </c>
       <c r="B13" t="s">
-        <v>142</v>
+        <v>91</v>
       </c>
       <c r="C13">
-        <v>0.056552613116585347</v>
+        <v>0.47933801402904541</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>143</v>
+        <v>92</v>
       </c>
       <c r="B14" t="s">
-        <v>144</v>
+        <v>93</v>
       </c>
       <c r="C14">
-        <v>0.061636272656695523</v>
+        <v>0.00014503412337480001</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>145</v>
+        <v>94</v>
       </c>
       <c r="B15" t="s">
-        <v>146</v>
+        <v>95</v>
       </c>
       <c r="C15">
-        <v>0.085274382777764654</v>
+        <v>0.0028310528606146001</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>147</v>
+        <v>96</v>
       </c>
       <c r="B16" t="s">
-        <v>148</v>
-      </c>
-      <c r="C16"/>
+        <v>97</v>
+      </c>
+      <c r="C16">
+        <v>0.0101844945559703</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>149</v>
-      </c>
-      <c r="B17" t="s">
-        <v>150</v>
+        <v>98</v>
       </c>
       <c r="C17">
-        <v>0.77365000785331983</v>
+        <v>0.0002826496369742</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>151</v>
+        <v>99</v>
       </c>
       <c r="B18" t="s">
-        <v>152</v>
-      </c>
-      <c r="C18">
-        <v>0.0052165302139223413</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>153</v>
+        <v>101</v>
       </c>
       <c r="B19" t="s">
-        <v>154</v>
-      </c>
-      <c r="C19">
-        <v>0.0024322786700245744</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>155</v>
+        <v>103</v>
       </c>
       <c r="B20" t="s">
-        <v>156</v>
-      </c>
-      <c r="C20">
-        <v>0.054588998957051348</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>157</v>
+        <v>105</v>
       </c>
       <c r="B21" t="s">
-        <v>158</v>
-      </c>
-      <c r="C21">
-        <v>0.070037909062677831</v>
+        <v>106</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>159</v>
+        <v>107</v>
       </c>
       <c r="B22" t="s">
-        <v>160</v>
-      </c>
-      <c r="C22">
-        <v>0.0068240640876526381</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>161</v>
+        <v>109</v>
       </c>
       <c r="B23" t="s">
-        <v>162</v>
+        <v>110</v>
       </c>
       <c r="C23">
-        <v>0.99385976219874372</v>
+        <v>0.2208438646282479</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>163</v>
+        <v>111</v>
       </c>
       <c r="B24" t="s">
-        <v>164</v>
+        <v>112</v>
       </c>
       <c r="C24">
-        <v>0.59571836366003494</v>
+        <v>0.1310905020089069</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>113</v>
+      </c>
+      <c r="B25" t="s">
+        <v>114</v>
+      </c>
+      <c r="C25">
+        <v>4.3704862418200001e-07</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>165</v>
+        <v>115</v>
       </c>
       <c r="B26" t="s">
-        <v>166</v>
+        <v>116</v>
       </c>
       <c r="C26">
-        <v>2.31795626319e-13</v>
+        <v>5.6407893339e-06</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>117</v>
+      </c>
+      <c r="B27" t="s">
+        <v>118</v>
+      </c>
+      <c r="C27">
+        <v>0.00076361063500770003</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>119</v>
+      </c>
+      <c r="B28" t="s">
+        <v>120</v>
+      </c>
+      <c r="C28">
+        <v>3.4435466830600002e-06</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>121</v>
+      </c>
+      <c r="B29" t="s">
+        <v>122</v>
+      </c>
+      <c r="C29">
+        <v>0.52401780687608612</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>123</v>
+      </c>
+      <c r="B30" t="s">
+        <v>124</v>
+      </c>
+      <c r="C30">
+        <v>0.14909696686314861</v>
       </c>
     </row>
   </sheetData>
@@ -2470,43 +2340,317 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C26"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2">
+        <v>0.1002074182866047</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C3"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C4">
+        <v>0.055103058469374036</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C5">
+        <v>0.029033502141470782</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>135</v>
+      </c>
+      <c r="B6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C6">
+        <v>4.7321178266967067e-06</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>137</v>
+      </c>
+      <c r="B7" t="s">
+        <v>138</v>
+      </c>
+      <c r="C7">
+        <v>0.45929648773349718</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B8" t="s">
+        <v>140</v>
+      </c>
+      <c r="C8">
+        <v>0.0010867068304195367</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>141</v>
+      </c>
+      <c r="B9" t="s">
+        <v>142</v>
+      </c>
+      <c r="C9">
+        <v>0.04208649098639583</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>143</v>
+      </c>
+      <c r="B10" t="s">
+        <v>144</v>
+      </c>
+      <c r="C10">
+        <v>0.35067052824028377</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>145</v>
+      </c>
+      <c r="C11">
+        <v>0.29149630622275757</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>146</v>
+      </c>
+      <c r="B12" t="s">
+        <v>147</v>
+      </c>
+      <c r="C12">
+        <v>0.032963613244158675</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>148</v>
+      </c>
+      <c r="B13" t="s">
+        <v>149</v>
+      </c>
+      <c r="C13">
+        <v>0.056552613116585597</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>150</v>
+      </c>
+      <c r="B14" t="s">
+        <v>151</v>
+      </c>
+      <c r="C14">
+        <v>0.061636272656695662</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>152</v>
+      </c>
+      <c r="B15" t="s">
+        <v>153</v>
+      </c>
+      <c r="C15">
+        <v>0.085274382777764654</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>154</v>
+      </c>
+      <c r="B16" t="s">
+        <v>155</v>
+      </c>
+      <c r="C16"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>156</v>
+      </c>
+      <c r="B17" t="s">
+        <v>157</v>
+      </c>
+      <c r="C17">
+        <v>0.77365000785331939</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>158</v>
+      </c>
+      <c r="B18" t="s">
+        <v>159</v>
+      </c>
+      <c r="C18">
+        <v>0.0052165302139223413</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>160</v>
+      </c>
+      <c r="B19" t="s">
+        <v>161</v>
+      </c>
+      <c r="C19">
+        <v>0.0024322786700245627</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>162</v>
+      </c>
+      <c r="B20" t="s">
+        <v>163</v>
+      </c>
+      <c r="C20">
+        <v>0.054588998957051202</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>164</v>
+      </c>
+      <c r="B21" t="s">
+        <v>165</v>
+      </c>
+      <c r="C21">
+        <v>0.070037909062677775</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>166</v>
+      </c>
+      <c r="B22" t="s">
+        <v>167</v>
+      </c>
+      <c r="C22">
+        <v>0.0068240640876526043</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>168</v>
+      </c>
+      <c r="B23" t="s">
+        <v>169</v>
+      </c>
+      <c r="C23">
+        <v>0.99385976219874372</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>170</v>
+      </c>
+      <c r="B24" t="s">
+        <v>171</v>
+      </c>
+      <c r="C24">
+        <v>0.59571836366003483</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>172</v>
+      </c>
+      <c r="B26" t="s">
+        <v>173</v>
+      </c>
+      <c r="C26">
+        <v>2.31795626319e-13</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C28"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="B1" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="C1" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="C2">
-        <v>0.085004121872091304</v>
+        <v>0.085004121872089999</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="B3" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="C3"/>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="B4" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="C4">
         <v>0.97389080393699001</v>
@@ -2514,76 +2658,76 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="B5" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="C5">
-        <v>0.87944926438836957</v>
+        <v>0.87944926438836935</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="B6" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="C6">
-        <v>0.17582780013652397</v>
+        <v>0.17582780013652335</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="B7" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="C7">
-        <v>0.10813407927520755</v>
+        <v>0.10813407927520749</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="B8" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="C8">
-        <v>5.1684037516812018e-06</v>
+        <v>5.1684037516811171e-06</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="B9" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="C9">
-        <v>0.34360973566103936</v>
+        <v>0.34360973566103958</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="B10" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="C10">
-        <v>0.00048672243499295835</v>
+        <v>0.00048672243499295391</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="B11" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="C11">
         <v>0.039672702352655721</v>
@@ -2591,10 +2735,10 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="B12" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="C12">
         <v>0.39121086727257182</v>
@@ -2602,7 +2746,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="C13">
         <v>0.44254089302598421</v>
@@ -2610,96 +2754,96 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
       <c r="B14" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
       <c r="C14">
-        <v>0.078614285938276476</v>
+        <v>0.078614285938276379</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="B15" t="s">
-        <v>195</v>
+        <v>202</v>
       </c>
       <c r="C15">
-        <v>0.080178100318648277</v>
+        <v>0.080178100318648318</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
       <c r="B16" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="C16">
-        <v>0.090296367319321252</v>
+        <v>0.090296367319321127</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="B17" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="C17">
-        <v>0.12370273934868546</v>
+        <v>0.12370273934868534</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="B18" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="C18"/>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="B19" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="C19">
-        <v>0.85455876739642822</v>
+        <v>0.85455876739642778</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="B20" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="C20">
-        <v>0.0055995659718764907</v>
+        <v>0.0055995659718765176</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="B21" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
       <c r="C21">
-        <v>0.0026403576379782018</v>
+        <v>0.0026403576379781918</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>208</v>
+        <v>215</v>
       </c>
       <c r="B22" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
       <c r="C22">
         <v>0.02873637921324974</v>
@@ -2707,32 +2851,32 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="B23" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="C23">
-        <v>0.054726723598558749</v>
+        <v>0.054726723598558784</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>212</v>
+        <v>219</v>
       </c>
       <c r="B24" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="C24">
-        <v>0.0087485335006279499</v>
+        <v>0.0087485335006279152</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="B25" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
       <c r="C25">
         <v>0.97952903018183424</v>
@@ -2740,24 +2884,24 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>216</v>
+        <v>223</v>
       </c>
       <c r="B26" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
       <c r="C26">
-        <v>0.51554369828354973</v>
+        <v>0.51554369828354951</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
       <c r="B28" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
       <c r="C28">
-        <v>0.0015250445038728</v>
+        <v>0.0015250445038728999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>